<commit_message>
Semantic analysis code and results
</commit_message>
<xml_diff>
--- a/analysis/pre_gemini_data/Participant100/Task1_Hard.xlsx
+++ b/analysis/pre_gemini_data/Participant100/Task1_Hard.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>arg10</t>
   </si>
@@ -106,7 +106,7 @@
     <t>Conditional</t>
   </si>
   <si>
-    <t>Body</t>
+    <t>condBody1</t>
   </si>
   <si>
     <t>Declaration</t>
@@ -121,7 +121,10 @@
     <t>loop</t>
   </si>
   <si>
-    <t>Loop</t>
+    <t>Loopbod</t>
+  </si>
+  <si>
+    <t>condBody2</t>
   </si>
   <si>
     <t>method1</t>
@@ -201,7 +204,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +215,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -248,16 +257,16 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -746,66 +755,66 @@
         <v>35</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AN1" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AO1" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AQ1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AS1" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AT1" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AU1" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AV1" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AW1" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AX1" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AY1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="BB1" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -945,9 +954,9 @@
       <c r="BC2" s="1"/>
       <c r="BD2" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1087,9 +1096,9 @@
       <c r="BC3" s="1"/>
       <c r="BD3" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1229,9 +1238,9 @@
       <c r="BC4" s="1"/>
       <c r="BD4" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1371,9 +1380,9 @@
       <c r="BC5" s="1"/>
       <c r="BD5" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1513,9 +1522,9 @@
       <c r="BC6" s="1"/>
       <c r="BD6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1590,7 +1599,7 @@
       <c r="AD7" s="5">
         <v>266.94</v>
       </c>
-      <c r="AE7" s="3"/>
+      <c r="AE7" s="2"/>
       <c r="AF7" s="5">
         <v>224.82</v>
       </c>

</xml_diff>